<commit_message>
docs(Setup): Add more docs and modify feat mng file
</commit_message>
<xml_diff>
--- a/Static/Docs/FeatManagementDoc.xlsx
+++ b/Static/Docs/FeatManagementDoc.xlsx
@@ -8,21 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CODE_PROJECTS\ASPNET_CORE_VSA_Template\Static\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AA3CCC9-34C3-46CE-8CEF-BEFAFEB8EEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C03C9D-BF38-47EC-BA39-6B2A394A3899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Project Tracking" sheetId="1" r:id="rId1"/>
-    <sheet name="Setting" sheetId="2" r:id="rId2"/>
+    <sheet name="Features Tracking" sheetId="1" r:id="rId1"/>
+    <sheet name="External Module Tracking" sheetId="3" r:id="rId2"/>
+    <sheet name="Setting" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="CategoryList">Setting!#REF!</definedName>
-    <definedName name="ColumnTitle1">'Project Tracking'!$B$4</definedName>
+    <definedName name="ColumnTitle1" localSheetId="1">'External Module Tracking'!$B$4</definedName>
+    <definedName name="ColumnTitle1">'Features Tracking'!$B$4</definedName>
     <definedName name="ColumnTitle2">#REF!</definedName>
     <definedName name="EmployeeList">Setting!$B$5:$B$5</definedName>
-    <definedName name="FlagPercent">'Project Tracking'!$D$2</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project Tracking'!$4:$4</definedName>
+    <definedName name="FlagPercent" localSheetId="1">'External Module Tracking'!$D$2</definedName>
+    <definedName name="FlagPercent">'Features Tracking'!$D$2</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'External Module Tracking'!$4:$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Features Tracking'!$4:$4</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="92">
   <si>
     <t>Biểu tượng cờ cho Công việc Thực tế Trên/Dưới (theo giờ)</t>
   </si>
@@ -50,9 +54,6 @@
     <t>Biểu tượng cờ cho Khoảng thời gian Thực tế Trên/Dưới (theo ngày)</t>
   </si>
   <si>
-    <t>Features</t>
-  </si>
-  <si>
     <t>F1</t>
   </si>
   <si>
@@ -237,6 +238,90 @@
   </si>
   <si>
     <t>Note</t>
+  </si>
+  <si>
+    <t>Is delivered</t>
+  </si>
+  <si>
+    <t>CODING STATUS</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Just a part</t>
+  </si>
+  <si>
+    <t>Half of progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing progress </t>
+  </si>
+  <si>
+    <t>Coding progress</t>
+  </si>
+  <si>
+    <t>So far so good</t>
+  </si>
+  <si>
+    <t>TESTING STATUS</t>
+  </si>
+  <si>
+    <t>Not yet</t>
+  </si>
+  <si>
+    <t>Just test some part</t>
+  </si>
+  <si>
+    <t>More tests have been done</t>
+  </si>
+  <si>
+    <t>IS DELIVERED</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Has delivered</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Has not delivered</t>
+  </si>
+  <si>
+    <t>Features Tracking</t>
+  </si>
+  <si>
+    <t>External Module Tracking</t>
+  </si>
+  <si>
+    <t>FA1</t>
+  </si>
+  <si>
+    <t>FA2</t>
+  </si>
+  <si>
+    <t>FA3</t>
+  </si>
+  <si>
+    <t>FA4</t>
+  </si>
+  <si>
+    <t>Integrate snowflake Id generator library for generating snowflake Id</t>
+  </si>
+  <si>
+    <t>Intergrate Nswag library for swagger</t>
+  </si>
+  <si>
+    <t>Integrate JWT authentication library for JWT auth</t>
+  </si>
+  <si>
+    <t>Integrate with postgressql database using NGPSQL library and also include ASP NET Core Identity database system</t>
   </si>
 </sst>
 </file>
@@ -624,9 +709,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -636,7 +718,10 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -658,7 +743,7 @@
     <cellStyle name="Title" xfId="9" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Văn bản" xfId="5" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="62">
     <dxf>
       <font>
         <b/>
@@ -675,55 +760,80 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Tahoma"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Tahoma"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Tahoma"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Tahoma"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="none"/>
-      </font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.89989928891872917"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.89989928891872917"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.89989928891872917"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1061,6 +1171,649 @@
         <right/>
         <top/>
         <bottom style="thin">
+          <color rgb="FFF8943F"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.89989928891872917"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.89989928891872917"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.89989928891872917"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.89989928891872917"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.89989928891872917"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;Over/Under flag&quot;;&quot;&quot;;&quot;&quot;"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.89989928891872917"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;Over/Under flag&quot;;&quot;&quot;;&quot;&quot;"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.89992980742820516"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.89992980742820516"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.89989928891872917"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.89989928891872917"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.89992980742820516"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.89992980742820516"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.89989928891872917"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.89989928891872917"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.89989928891872917"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
           <color theme="9"/>
         </bottom>
       </border>
@@ -1130,8 +1883,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium2">
     <tableStyle name="Kiểu Bảng Tùy chỉnh" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="24"/>
-      <tableStyleElement type="headerRow" dxfId="23"/>
+      <tableStyleElement type="wholeTable" dxfId="61"/>
+      <tableStyleElement type="headerRow" dxfId="60"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1146,42 +1899,127 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Bộ_theo_dõi_Dự_án" displayName="Bộ_theo_dõi_Dự_án" ref="B4:O25" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
-  <autoFilter ref="B4:O25" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Feature" dataDxfId="19" dataCellStyle="Văn bản"/>
-    <tableColumn id="16" xr3:uid="{DCA8AFC4-B1D9-3C43-B18E-F50FCCFC9A7A}" name="Description" dataDxfId="18" dataCellStyle="Văn bản"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Author" dataDxfId="17" dataCellStyle="Văn bản"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Planned start day" dataDxfId="16" dataCellStyle="Ngày"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Planned end day" dataDxfId="15" dataCellStyle="Ngày"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Planned amount of time" dataDxfId="14" dataCellStyle="Số"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Planned number of days" dataDxfId="13" dataCellStyle="Khoảng thời gian dự kiến">
-      <calculatedColumnFormula>IF(COUNTA('Project Tracking'!$E5,'Project Tracking'!$F5)&lt;&gt;2,"",DAYS360('Project Tracking'!$E5,'Project Tracking'!$F5,FALSE))</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Bộ_theo_dõi_Dự_án" displayName="Bộ_theo_dõi_Dự_án" ref="B4:R25" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
+  <autoFilter ref="B4:R25" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Feature" dataDxfId="56" dataCellStyle="Văn bản"/>
+    <tableColumn id="16" xr3:uid="{DCA8AFC4-B1D9-3C43-B18E-F50FCCFC9A7A}" name="Description" dataDxfId="55" dataCellStyle="Văn bản"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Author" dataDxfId="54" dataCellStyle="Văn bản"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Planned start day" dataDxfId="53" dataCellStyle="Ngày"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Planned end day" dataDxfId="52" dataCellStyle="Ngày"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Planned amount of time" dataDxfId="51" dataCellStyle="Số"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Planned number of days" dataDxfId="50" dataCellStyle="Khoảng thời gian dự kiến">
+      <calculatedColumnFormula>IF(COUNTA('Features Tracking'!$E5,'Features Tracking'!$F5)&lt;&gt;2,"",DAYS360('Features Tracking'!$E5,'Features Tracking'!$F5,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Actual start day" dataDxfId="12" dataCellStyle="Ngày bắt đầu Thực tế"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Actual end day" dataDxfId="11" dataCellStyle="Ngày"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Biểu tượng cờ cho Công việc Thực tế Trên/Dưới (theo giờ)" dataDxfId="10" dataCellStyle="Gắn cờ">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Actual start day" dataDxfId="49" dataCellStyle="Ngày bắt đầu Thực tế"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Actual end day" dataDxfId="48" dataCellStyle="Ngày"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Biểu tượng cờ cho Công việc Thực tế Trên/Dưới (theo giờ)" dataDxfId="47" dataCellStyle="Gắn cờ">
       <calculatedColumnFormula>IFERROR(IF(Bộ_theo_dõi_Dự_án[[#This Row],[Actual amount of time]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án[[#This Row],[Actual amount of time]]-Bộ_theo_dõi_Dự_án[[#This Row],[Planned amount of time]])/Bộ_theo_dõi_Dự_án[[#This Row],[Planned amount of time]])&gt;FlagPercent,1,0)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Actual amount of time" dataDxfId="9" dataCellStyle="Số"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Biểu tượng cờ cho Khoảng thời gian Thực tế Trên/Dưới (theo ngày)" dataDxfId="8" dataCellStyle="Gắn cờ">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Actual amount of time" dataDxfId="46" dataCellStyle="Số"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Biểu tượng cờ cho Khoảng thời gian Thực tế Trên/Dưới (theo ngày)" dataDxfId="45" dataCellStyle="Gắn cờ">
       <calculatedColumnFormula>IFERROR(IF(Bộ_theo_dõi_Dự_án[[#This Row],[Actual number of days]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án[[#This Row],[Actual number of days]]-Bộ_theo_dõi_Dự_án[[#This Row],[Planned number of days]])/Bộ_theo_dõi_Dự_án[[#This Row],[Planned number of days]])&gt;FlagPercent,1,0)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Actual number of days" dataDxfId="7" dataCellStyle="Cột Xám">
-      <calculatedColumnFormula>IF(COUNTA('Project Tracking'!$I5,'Project Tracking'!$J5)&lt;&gt;2,"",DAYS360('Project Tracking'!$I5,'Project Tracking'!$J5,FALSE))</calculatedColumnFormula>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Actual number of days" dataDxfId="44" dataCellStyle="Cột Xám">
+      <calculatedColumnFormula>IF(COUNTA('Features Tracking'!$I5,'Features Tracking'!$J5)&lt;&gt;2,"",DAYS360('Features Tracking'!$I5,'Features Tracking'!$J5,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Note" dataDxfId="6" dataCellStyle="Văn bản"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Coding progress" dataDxfId="43" dataCellStyle="Văn bản"/>
+    <tableColumn id="17" xr3:uid="{C95ED1E6-E0DC-41DB-A4AE-65DED2862E22}" name="Testing progress " dataDxfId="42" dataCellStyle="Văn bản"/>
+    <tableColumn id="18" xr3:uid="{E05DEF6E-2723-4DE9-901C-8F3E946B0B43}" name="Is delivered" dataDxfId="41" dataCellStyle="Văn bản"/>
+    <tableColumn id="19" xr3:uid="{D97DD52F-440B-4DAD-9594-12C53408A9FE}" name="Note" dataDxfId="40" dataCellStyle="Văn bản"/>
   </tableColumns>
   <tableStyleInfo name="Kiểu Bảng Tùy chỉnh" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="CategoryAndEmployeeTable" displayName="CategoryAndEmployeeTable" ref="B4:C5" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" dataCellStyle="Văn bản">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DE3F41EF-04E2-414C-85F0-7851A4486493}" name="Bộ_theo_dõi_Dự_án7" displayName="Bộ_theo_dõi_Dự_án7" ref="B4:R8" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
+  <autoFilter ref="B4:R8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{3FD728DA-0611-40C3-911F-3A0A6A932314}" name="Feature" dataDxfId="20" dataCellStyle="Văn bản"/>
+    <tableColumn id="16" xr3:uid="{7E120945-28CF-4A07-922F-86D69A4D4E47}" name="Description" dataDxfId="19" dataCellStyle="Văn bản"/>
+    <tableColumn id="3" xr3:uid="{D1DFF380-08BA-48FA-8197-DD842353F1B1}" name="Author" dataDxfId="18" dataCellStyle="Văn bản"/>
+    <tableColumn id="4" xr3:uid="{8994769E-822B-4AE7-918D-F222AC0C376A}" name="Planned start day" dataDxfId="17" dataCellStyle="Ngày"/>
+    <tableColumn id="5" xr3:uid="{9C29F9F6-6121-4BD4-9D12-EF9D6ECA95AD}" name="Planned end day" dataDxfId="16" dataCellStyle="Ngày"/>
+    <tableColumn id="6" xr3:uid="{BE35B198-A475-4774-89FB-47CD793A59EB}" name="Planned amount of time" dataDxfId="15" dataCellStyle="Số"/>
+    <tableColumn id="7" xr3:uid="{D7B64D18-F61D-4357-8C3E-EAA5C054843F}" name="Planned number of days" dataDxfId="14" dataCellStyle="Khoảng thời gian dự kiến">
+      <calculatedColumnFormula>IF(COUNTA('External Module Tracking'!$E5,'External Module Tracking'!$F5)&lt;&gt;2,"",DAYS360('External Module Tracking'!$E5,'External Module Tracking'!$F5,FALSE))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{F5AA1398-9B37-406D-85DF-29F6C53BC47B}" name="Actual start day" dataDxfId="13" dataCellStyle="Ngày bắt đầu Thực tế"/>
+    <tableColumn id="9" xr3:uid="{DC277F4C-AC1D-4E62-81FD-14C9D876571A}" name="Actual end day" dataDxfId="12" dataCellStyle="Ngày"/>
+    <tableColumn id="10" xr3:uid="{65B58180-4994-498E-B39B-D2C4A3E03F8E}" name="Biểu tượng cờ cho Công việc Thực tế Trên/Dưới (theo giờ)" dataDxfId="11" dataCellStyle="Gắn cờ">
+      <calculatedColumnFormula>IFERROR(IF(Bộ_theo_dõi_Dự_án7[[#This Row],[Actual amount of time]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án7[[#This Row],[Actual amount of time]]-Bộ_theo_dõi_Dự_án7[[#This Row],[Planned amount of time]])/Bộ_theo_dõi_Dự_án7[[#This Row],[Planned amount of time]])&gt;FlagPercent,1,0)),"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{7B6587C5-5E19-4B8B-A967-BA353FD7FF2B}" name="Actual amount of time" dataDxfId="10" dataCellStyle="Số"/>
+    <tableColumn id="12" xr3:uid="{08F4CEE2-9B6A-4E8B-A816-D757A1BF7895}" name="Biểu tượng cờ cho Khoảng thời gian Thực tế Trên/Dưới (theo ngày)" dataDxfId="9" dataCellStyle="Gắn cờ">
+      <calculatedColumnFormula>IFERROR(IF(Bộ_theo_dõi_Dự_án7[[#This Row],[Actual number of days]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án7[[#This Row],[Actual number of days]]-Bộ_theo_dõi_Dự_án7[[#This Row],[Planned number of days]])/Bộ_theo_dõi_Dự_án7[[#This Row],[Planned number of days]])&gt;FlagPercent,1,0)),"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{BAF32103-F7B5-436D-8AE0-681FB4D73D6D}" name="Actual number of days" dataDxfId="8" dataCellStyle="Cột Xám">
+      <calculatedColumnFormula>IF(COUNTA('External Module Tracking'!$I5,'External Module Tracking'!$J5)&lt;&gt;2,"",DAYS360('External Module Tracking'!$I5,'External Module Tracking'!$J5,FALSE))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{81756D77-36CB-480F-BC44-3AC9CDB78226}" name="Coding progress" dataDxfId="7" dataCellStyle="Văn bản"/>
+    <tableColumn id="17" xr3:uid="{2F36C5EC-C0EB-4E32-809E-89FEA0ED345B}" name="Testing progress " dataDxfId="6" dataCellStyle="Văn bản"/>
+    <tableColumn id="18" xr3:uid="{A39AEEFA-D05D-42F6-9A76-73F3EAD8B373}" name="Is delivered" dataDxfId="5" dataCellStyle="Văn bản"/>
+    <tableColumn id="19" xr3:uid="{9EF765EB-23B7-4BF9-BC94-686CEEC3D74F}" name="Note" dataDxfId="4" dataCellStyle="Văn bản"/>
+  </tableColumns>
+  <tableStyleInfo name="Kiểu Bảng Tùy chỉnh" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="CategoryAndEmployeeTable" displayName="CategoryAndEmployeeTable" ref="B4:C5" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" dataCellStyle="Văn bản">
   <autoFilter ref="B4:C5" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Nickname" dataDxfId="3" dataCellStyle="Văn bản"/>
-    <tableColumn id="4" xr3:uid="{56E33E93-7B93-4F4E-A6E2-1E65C6E28E25}" name="Full Name" dataDxfId="2" dataCellStyle="Văn bản"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Nickname" dataDxfId="37" dataCellStyle="Văn bản"/>
+    <tableColumn id="4" xr3:uid="{56E33E93-7B93-4F4E-A6E2-1E65C6E28E25}" name="Full Name" dataDxfId="36" dataCellStyle="Văn bản"/>
+  </tableColumns>
+  <tableStyleInfo name="Kiểu Bảng Tùy chỉnh" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altTextSummary="Danh sách danh mục và nhân viên được dùng trong danh sách chọn thả xuống xác thực dữ liệu Danh mục và Nhân viên trên trang tính Bộ theo dõi Dự án. Sử dụng các cột này để tùy chỉnh các mục trong từng danh sách. Danh sách không cần có cùng một số mục"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C65FBD61-8562-45B3-942E-0C90707F4062}" name="CategoryAndEmployeeTable3" displayName="CategoryAndEmployeeTable3" ref="F4:G9" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" dataCellStyle="Văn bản">
+  <autoFilter ref="F4:G9" xr:uid="{C65FBD61-8562-45B3-942E-0C90707F4062}"/>
+  <tableColumns count="2">
+    <tableColumn id="2" xr3:uid="{56DEA1AD-EA6F-4FC2-AE9C-87317D88B274}" name="Status" dataDxfId="33" dataCellStyle="Văn bản"/>
+    <tableColumn id="4" xr3:uid="{AFD8BD1A-C789-4F12-AB32-B4219CAD81E4}" name="Description" dataDxfId="32" dataCellStyle="Văn bản"/>
+  </tableColumns>
+  <tableStyleInfo name="Kiểu Bảng Tùy chỉnh" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altTextSummary="Danh sách danh mục và nhân viên được dùng trong danh sách chọn thả xuống xác thực dữ liệu Danh mục và Nhân viên trên trang tính Bộ theo dõi Dự án. Sử dụng các cột này để tùy chỉnh các mục trong từng danh sách. Danh sách không cần có cùng một số mục"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3C3F336A-FEB0-45A9-8AF4-ED9B6CC3A338}" name="CategoryAndEmployeeTable35" displayName="CategoryAndEmployeeTable35" ref="I4:J9" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" dataCellStyle="Văn bản">
+  <autoFilter ref="I4:J9" xr:uid="{3C3F336A-FEB0-45A9-8AF4-ED9B6CC3A338}"/>
+  <tableColumns count="2">
+    <tableColumn id="2" xr3:uid="{957A9D09-1FF4-4DBA-833C-7361C5F0A9B1}" name="Status" dataDxfId="29" dataCellStyle="Văn bản"/>
+    <tableColumn id="4" xr3:uid="{7B47179B-393C-46D7-971A-6BAA06BE542C}" name="Description" dataDxfId="28" dataCellStyle="Văn bản"/>
+  </tableColumns>
+  <tableStyleInfo name="Kiểu Bảng Tùy chỉnh" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altTextSummary="Danh sách danh mục và nhân viên được dùng trong danh sách chọn thả xuống xác thực dữ liệu Danh mục và Nhân viên trên trang tính Bộ theo dõi Dự án. Sử dụng các cột này để tùy chỉnh các mục trong từng danh sách. Danh sách không cần có cùng một số mục"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F3179982-F55E-4720-B2E2-80FABD0E8CF9}" name="CategoryAndEmployeeTable356" displayName="CategoryAndEmployeeTable356" ref="L4:M6" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" dataCellStyle="Văn bản">
+  <autoFilter ref="L4:M6" xr:uid="{F3179982-F55E-4720-B2E2-80FABD0E8CF9}"/>
+  <tableColumns count="2">
+    <tableColumn id="2" xr3:uid="{DEF535F2-87F7-4CE2-B8BB-4B0CBC380B75}" name="Status" dataDxfId="25" dataCellStyle="Văn bản"/>
+    <tableColumn id="4" xr3:uid="{448EEB41-DAAA-4520-82AD-B523FDCC6E07}" name="Description" dataDxfId="24" dataCellStyle="Văn bản"/>
   </tableColumns>
   <tableStyleInfo name="Kiểu Bảng Tùy chỉnh" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1423,12 +2261,12 @@
     <tabColor theme="9"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1443,80 +2281,92 @@
     <col min="12" max="12" width="14.09765625" style="1" customWidth="1"/>
     <col min="13" max="13" width="2.796875" style="1" customWidth="1"/>
     <col min="14" max="14" width="14.3984375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="25.59765625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="2.69921875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="1"/>
+    <col min="15" max="15" width="15.796875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.09765625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15.296875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21.3984375" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="24" t="s">
-        <v>21</v>
+      <c r="C2" s="23" t="s">
+        <v>20</v>
       </c>
       <c r="D2" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:15" ht="54.9" customHeight="1" x14ac:dyDescent="0.25">
+        <f>COUNTIF(Q5:Q25,"Yes")/COUNTA(Q5:Q25)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:19" ht="54.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>19</v>
-      </c>
       <c r="G4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" s="10" t="s">
+      <c r="J4" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="K4" s="11" t="s">
         <v>0</v>
       </c>
       <c r="L4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="M4" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="N4" s="8" t="s">
+      <c r="O4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="R4" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="O4" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="13">
         <v>45667</v>
@@ -1528,16 +2378,16 @@
         <v>4</v>
       </c>
       <c r="H5" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E5,'Project Tracking'!$F5)&lt;&gt;2,"",DAYS360('Project Tracking'!$E5,'Project Tracking'!$F5,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E5,'Features Tracking'!$F5)&lt;&gt;2,"",DAYS360('Features Tracking'!$E5,'Features Tracking'!$F5,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I5" s="16">
         <f ca="1">TODAY()-65</f>
-        <v>45630</v>
+        <v>45631</v>
       </c>
       <c r="J5" s="13">
         <f ca="1">TODAY()</f>
-        <v>45695</v>
+        <v>45696</v>
       </c>
       <c r="K5" s="17">
         <f>IFERROR(IF(Bộ_theo_dõi_Dự_án[[#This Row],[Actual amount of time]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án[[#This Row],[Actual amount of time]]-Bộ_theo_dõi_Dự_án[[#This Row],[Planned amount of time]])/Bộ_theo_dõi_Dự_án[[#This Row],[Planned amount of time]])&gt;FlagPercent,1,0)),"")</f>
@@ -1551,20 +2401,30 @@
         <v>1</v>
       </c>
       <c r="N5" s="18">
-        <f ca="1">IF(COUNTA('Project Tracking'!$I5,'Project Tracking'!$J5)&lt;&gt;2,"",DAYS360('Project Tracking'!$I5,'Project Tracking'!$J5,FALSE))</f>
+        <f ca="1">IF(COUNTA('Features Tracking'!$I5,'Features Tracking'!$J5)&lt;&gt;2,"",DAYS360('Features Tracking'!$I5,'Features Tracking'!$J5,FALSE))</f>
         <v>63</v>
       </c>
-      <c r="O5" s="12"/>
-    </row>
-    <row r="6" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O5" s="27">
+        <v>1</v>
+      </c>
+      <c r="P5" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R5" s="21"/>
+      <c r="S5" s="12"/>
+    </row>
+    <row r="6" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="13">
         <v>45667</v>
@@ -1576,16 +2436,16 @@
         <v>4</v>
       </c>
       <c r="H6" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E6,'Project Tracking'!$F6)&lt;&gt;2,"",DAYS360('Project Tracking'!$E6,'Project Tracking'!$F6,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E6,'Features Tracking'!$F6)&lt;&gt;2,"",DAYS360('Features Tracking'!$E6,'Features Tracking'!$F6,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I6" s="16">
         <f ca="1">TODAY()-41</f>
-        <v>45654</v>
+        <v>45655</v>
       </c>
       <c r="J6" s="13">
         <f ca="1">TODAY()-7</f>
-        <v>45688</v>
+        <v>45689</v>
       </c>
       <c r="K6" s="17">
         <f>IFERROR(IF(Bộ_theo_dõi_Dự_án[[#This Row],[Actual amount of time]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án[[#This Row],[Actual amount of time]]-Bộ_theo_dõi_Dự_án[[#This Row],[Planned amount of time]])/Bộ_theo_dõi_Dự_án[[#This Row],[Planned amount of time]])&gt;FlagPercent,1,0)),"")</f>
@@ -1599,20 +2459,30 @@
         <v>0</v>
       </c>
       <c r="N6" s="18">
-        <f ca="1">IF(COUNTA('Project Tracking'!$I6,'Project Tracking'!$J6)&lt;&gt;2,"",DAYS360('Project Tracking'!$I6,'Project Tracking'!$J6,FALSE))</f>
-        <v>33</v>
-      </c>
-      <c r="O6" s="12"/>
-    </row>
-    <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <f ca="1">IF(COUNTA('Features Tracking'!$I6,'Features Tracking'!$J6)&lt;&gt;2,"",DAYS360('Features Tracking'!$I6,'Features Tracking'!$J6,FALSE))</f>
+        <v>32</v>
+      </c>
+      <c r="O6" s="27">
+        <v>1</v>
+      </c>
+      <c r="P6" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R6" s="21"/>
+      <c r="S6" s="12"/>
+    </row>
+    <row r="7" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="13">
         <v>45667</v>
@@ -1624,16 +2494,16 @@
         <v>4</v>
       </c>
       <c r="H7" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E7,'Project Tracking'!$F7)&lt;&gt;2,"",DAYS360('Project Tracking'!$E7,'Project Tracking'!$F7,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E7,'Features Tracking'!$F7)&lt;&gt;2,"",DAYS360('Features Tracking'!$E7,'Features Tracking'!$F7,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I7" s="16">
         <f ca="1">TODAY()-100</f>
-        <v>45595</v>
+        <v>45596</v>
       </c>
       <c r="J7" s="13">
         <f ca="1">TODAY()-27</f>
-        <v>45668</v>
+        <v>45669</v>
       </c>
       <c r="K7" s="17">
         <f>IFERROR(IF(Bộ_theo_dõi_Dự_án[[#This Row],[Actual amount of time]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án[[#This Row],[Actual amount of time]]-Bộ_theo_dõi_Dự_án[[#This Row],[Planned amount of time]])/Bộ_theo_dõi_Dự_án[[#This Row],[Planned amount of time]])&gt;FlagPercent,1,0)),"")</f>
@@ -1647,20 +2517,30 @@
         <v>1</v>
       </c>
       <c r="N7" s="18">
-        <f ca="1">IF(COUNTA('Project Tracking'!$I7,'Project Tracking'!$J7)&lt;&gt;2,"",DAYS360('Project Tracking'!$I7,'Project Tracking'!$J7,FALSE))</f>
-        <v>71</v>
-      </c>
-      <c r="O7" s="12"/>
-    </row>
-    <row r="8" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <f ca="1">IF(COUNTA('Features Tracking'!$I7,'Features Tracking'!$J7)&lt;&gt;2,"",DAYS360('Features Tracking'!$I7,'Features Tracking'!$J7,FALSE))</f>
+        <v>72</v>
+      </c>
+      <c r="O7" s="27">
+        <v>1</v>
+      </c>
+      <c r="P7" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R7" s="21"/>
+      <c r="S7" s="12"/>
+    </row>
+    <row r="8" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="13">
         <v>45667</v>
@@ -1672,16 +2552,16 @@
         <v>4</v>
       </c>
       <c r="H8" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E8,'Project Tracking'!$F8)&lt;&gt;2,"",DAYS360('Project Tracking'!$E8,'Project Tracking'!$F8,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E8,'Features Tracking'!$F8)&lt;&gt;2,"",DAYS360('Features Tracking'!$E8,'Features Tracking'!$F8,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I8" s="16">
         <f ca="1">TODAY()-90</f>
-        <v>45605</v>
+        <v>45606</v>
       </c>
       <c r="J8" s="13">
         <f ca="1">TODAY()-71</f>
-        <v>45624</v>
+        <v>45625</v>
       </c>
       <c r="K8" s="17">
         <f>IFERROR(IF(Bộ_theo_dõi_Dự_án[[#This Row],[Actual amount of time]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án[[#This Row],[Actual amount of time]]-Bộ_theo_dõi_Dự_án[[#This Row],[Planned amount of time]])/Bộ_theo_dõi_Dự_án[[#This Row],[Planned amount of time]])&gt;FlagPercent,1,0)),"")</f>
@@ -1695,20 +2575,30 @@
         <v>0</v>
       </c>
       <c r="N8" s="18">
-        <f ca="1">IF(COUNTA('Project Tracking'!$I8,'Project Tracking'!$J8)&lt;&gt;2,"",DAYS360('Project Tracking'!$I8,'Project Tracking'!$J8,FALSE))</f>
+        <f ca="1">IF(COUNTA('Features Tracking'!$I8,'Features Tracking'!$J8)&lt;&gt;2,"",DAYS360('Features Tracking'!$I8,'Features Tracking'!$J8,FALSE))</f>
         <v>19</v>
       </c>
-      <c r="O8" s="12"/>
-    </row>
-    <row r="9" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O8" s="27">
+        <v>1</v>
+      </c>
+      <c r="P8" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R8" s="21"/>
+      <c r="S8" s="12"/>
+    </row>
+    <row r="9" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="13">
         <v>45667</v>
@@ -1720,16 +2610,16 @@
         <v>4</v>
       </c>
       <c r="H9" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E9,'Project Tracking'!$F9)&lt;&gt;2,"",DAYS360('Project Tracking'!$E9,'Project Tracking'!$F9,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E9,'Features Tracking'!$F9)&lt;&gt;2,"",DAYS360('Features Tracking'!$E9,'Features Tracking'!$F9,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I9" s="16">
         <f ca="1">TODAY()-90</f>
-        <v>45605</v>
+        <v>45606</v>
       </c>
       <c r="J9" s="13">
         <f ca="1">TODAY()-44</f>
-        <v>45651</v>
+        <v>45652</v>
       </c>
       <c r="K9" s="17">
         <f>IFERROR(IF(Bộ_theo_dõi_Dự_án[[#This Row],[Actual amount of time]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án[[#This Row],[Actual amount of time]]-Bộ_theo_dõi_Dự_án[[#This Row],[Planned amount of time]])/Bộ_theo_dõi_Dự_án[[#This Row],[Planned amount of time]])&gt;FlagPercent,1,0)),"")</f>
@@ -1743,20 +2633,30 @@
         <v>0</v>
       </c>
       <c r="N9" s="18">
-        <f ca="1">IF(COUNTA('Project Tracking'!$I9,'Project Tracking'!$J9)&lt;&gt;2,"",DAYS360('Project Tracking'!$I9,'Project Tracking'!$J9,FALSE))</f>
+        <f ca="1">IF(COUNTA('Features Tracking'!$I9,'Features Tracking'!$J9)&lt;&gt;2,"",DAYS360('Features Tracking'!$I9,'Features Tracking'!$J9,FALSE))</f>
         <v>46</v>
       </c>
-      <c r="O9" s="12"/>
-    </row>
-    <row r="10" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O9" s="27">
+        <v>1</v>
+      </c>
+      <c r="P9" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R9" s="21"/>
+      <c r="S9" s="12"/>
+    </row>
+    <row r="10" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="13">
         <v>45667</v>
@@ -1768,16 +2668,16 @@
         <v>4</v>
       </c>
       <c r="H10" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E10,'Project Tracking'!$F10)&lt;&gt;2,"",DAYS360('Project Tracking'!$E10,'Project Tracking'!$F10,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E10,'Features Tracking'!$F10)&lt;&gt;2,"",DAYS360('Features Tracking'!$E10,'Features Tracking'!$F10,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I10" s="16">
         <f ca="1">TODAY()-60</f>
-        <v>45635</v>
+        <v>45636</v>
       </c>
       <c r="J10" s="13">
         <f ca="1">TODAY()-45</f>
-        <v>45650</v>
+        <v>45651</v>
       </c>
       <c r="K10" s="17">
         <f>IFERROR(IF(Bộ_theo_dõi_Dự_án[[#This Row],[Actual amount of time]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án[[#This Row],[Actual amount of time]]-Bộ_theo_dõi_Dự_án[[#This Row],[Planned amount of time]])/Bộ_theo_dõi_Dự_án[[#This Row],[Planned amount of time]])&gt;FlagPercent,1,0)),"")</f>
@@ -1791,20 +2691,30 @@
         <v>0</v>
       </c>
       <c r="N10" s="18">
-        <f ca="1">IF(COUNTA('Project Tracking'!$I10,'Project Tracking'!$J10)&lt;&gt;2,"",DAYS360('Project Tracking'!$I10,'Project Tracking'!$J10,FALSE))</f>
+        <f ca="1">IF(COUNTA('Features Tracking'!$I10,'Features Tracking'!$J10)&lt;&gt;2,"",DAYS360('Features Tracking'!$I10,'Features Tracking'!$J10,FALSE))</f>
         <v>15</v>
       </c>
-      <c r="O10" s="12"/>
-    </row>
-    <row r="11" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O10" s="27">
+        <v>1</v>
+      </c>
+      <c r="P10" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R10" s="21"/>
+      <c r="S10" s="12"/>
+    </row>
+    <row r="11" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" s="13">
         <v>45667</v>
@@ -1816,16 +2726,16 @@
         <v>4</v>
       </c>
       <c r="H11" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E11,'Project Tracking'!$F11)&lt;&gt;2,"",DAYS360('Project Tracking'!$E11,'Project Tracking'!$F11,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E11,'Features Tracking'!$F11)&lt;&gt;2,"",DAYS360('Features Tracking'!$E11,'Features Tracking'!$F11,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I11" s="16">
         <f ca="1">TODAY()-44</f>
-        <v>45651</v>
+        <v>45652</v>
       </c>
       <c r="J11" s="13">
         <f ca="1">TODAY()-15</f>
-        <v>45680</v>
+        <v>45681</v>
       </c>
       <c r="K11" s="17">
         <f>IFERROR(IF(Bộ_theo_dõi_Dự_án[[#This Row],[Actual amount of time]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án[[#This Row],[Actual amount of time]]-Bộ_theo_dõi_Dự_án[[#This Row],[Planned amount of time]])/Bộ_theo_dõi_Dự_án[[#This Row],[Planned amount of time]])&gt;FlagPercent,1,0)),"")</f>
@@ -1839,20 +2749,30 @@
         <v>0</v>
       </c>
       <c r="N11" s="18">
-        <f ca="1">IF(COUNTA('Project Tracking'!$I11,'Project Tracking'!$J11)&lt;&gt;2,"",DAYS360('Project Tracking'!$I11,'Project Tracking'!$J11,FALSE))</f>
+        <f ca="1">IF(COUNTA('Features Tracking'!$I11,'Features Tracking'!$J11)&lt;&gt;2,"",DAYS360('Features Tracking'!$I11,'Features Tracking'!$J11,FALSE))</f>
         <v>28</v>
       </c>
-      <c r="O11" s="12"/>
-    </row>
-    <row r="12" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O11" s="27">
+        <v>1</v>
+      </c>
+      <c r="P11" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R11" s="21"/>
+      <c r="S11" s="12"/>
+    </row>
+    <row r="12" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12" s="13">
         <v>45667</v>
@@ -1864,16 +2784,16 @@
         <v>4</v>
       </c>
       <c r="H12" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E12,'Project Tracking'!$F12)&lt;&gt;2,"",DAYS360('Project Tracking'!$E12,'Project Tracking'!$F12,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E12,'Features Tracking'!$F12)&lt;&gt;2,"",DAYS360('Features Tracking'!$E12,'Features Tracking'!$F12,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I12" s="16">
         <f ca="1">TODAY()-45</f>
-        <v>45650</v>
+        <v>45651</v>
       </c>
       <c r="J12" s="13">
         <f ca="1">TODAY()-5</f>
-        <v>45690</v>
+        <v>45691</v>
       </c>
       <c r="K12" s="17">
         <f>IFERROR(IF(Bộ_theo_dõi_Dự_án[[#This Row],[Actual amount of time]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án[[#This Row],[Actual amount of time]]-Bộ_theo_dõi_Dự_án[[#This Row],[Planned amount of time]])/Bộ_theo_dõi_Dự_án[[#This Row],[Planned amount of time]])&gt;FlagPercent,1,0)),"")</f>
@@ -1887,20 +2807,30 @@
         <v>0</v>
       </c>
       <c r="N12" s="18">
-        <f ca="1">IF(COUNTA('Project Tracking'!$I12,'Project Tracking'!$J12)&lt;&gt;2,"",DAYS360('Project Tracking'!$I12,'Project Tracking'!$J12,FALSE))</f>
+        <f ca="1">IF(COUNTA('Features Tracking'!$I12,'Features Tracking'!$J12)&lt;&gt;2,"",DAYS360('Features Tracking'!$I12,'Features Tracking'!$J12,FALSE))</f>
         <v>38</v>
       </c>
-      <c r="O12" s="12"/>
-    </row>
-    <row r="13" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O12" s="27">
+        <v>1</v>
+      </c>
+      <c r="P12" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R12" s="21"/>
+      <c r="S12" s="12"/>
+    </row>
+    <row r="13" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="13">
         <v>45667</v>
@@ -1912,7 +2842,7 @@
         <v>4</v>
       </c>
       <c r="H13" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E13,'Project Tracking'!$F13)&lt;&gt;2,"",DAYS360('Project Tracking'!$E13,'Project Tracking'!$F13,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E13,'Features Tracking'!$F13)&lt;&gt;2,"",DAYS360('Features Tracking'!$E13,'Features Tracking'!$F13,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I13" s="16">
@@ -1933,20 +2863,30 @@
         <v>0</v>
       </c>
       <c r="N13" s="18">
-        <f>IF(COUNTA('Project Tracking'!$I13,'Project Tracking'!$J13)&lt;&gt;2,"",DAYS360('Project Tracking'!$I13,'Project Tracking'!$J13,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$I13,'Features Tracking'!$J13)&lt;&gt;2,"",DAYS360('Features Tracking'!$I13,'Features Tracking'!$J13,FALSE))</f>
         <v>60</v>
       </c>
-      <c r="O13" s="12"/>
-    </row>
-    <row r="14" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O13" s="27">
+        <v>1</v>
+      </c>
+      <c r="P13" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R13" s="21"/>
+      <c r="S13" s="12"/>
+    </row>
+    <row r="14" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" s="13">
         <v>45667</v>
@@ -1958,7 +2898,7 @@
         <v>4</v>
       </c>
       <c r="H14" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E14,'Project Tracking'!$F14)&lt;&gt;2,"",DAYS360('Project Tracking'!$E14,'Project Tracking'!$F14,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E14,'Features Tracking'!$F14)&lt;&gt;2,"",DAYS360('Features Tracking'!$E14,'Features Tracking'!$F14,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I14" s="16">
@@ -1979,20 +2919,30 @@
         <v>0</v>
       </c>
       <c r="N14" s="18">
-        <f>IF(COUNTA('Project Tracking'!$I14,'Project Tracking'!$J14)&lt;&gt;2,"",DAYS360('Project Tracking'!$I14,'Project Tracking'!$J14,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$I14,'Features Tracking'!$J14)&lt;&gt;2,"",DAYS360('Features Tracking'!$I14,'Features Tracking'!$J14,FALSE))</f>
         <v>60</v>
       </c>
-      <c r="O14" s="23"/>
-    </row>
-    <row r="15" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O14" s="27">
+        <v>1</v>
+      </c>
+      <c r="P14" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R14" s="21"/>
+      <c r="S14" s="12"/>
+    </row>
+    <row r="15" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E15" s="13">
         <v>45667</v>
@@ -2004,7 +2954,7 @@
         <v>4</v>
       </c>
       <c r="H15" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E15,'Project Tracking'!$F15)&lt;&gt;2,"",DAYS360('Project Tracking'!$E15,'Project Tracking'!$F15,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E15,'Features Tracking'!$F15)&lt;&gt;2,"",DAYS360('Features Tracking'!$E15,'Features Tracking'!$F15,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I15" s="16">
@@ -2025,20 +2975,30 @@
         <v>0</v>
       </c>
       <c r="N15" s="18">
-        <f>IF(COUNTA('Project Tracking'!$I15,'Project Tracking'!$J15)&lt;&gt;2,"",DAYS360('Project Tracking'!$I15,'Project Tracking'!$J15,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$I15,'Features Tracking'!$J15)&lt;&gt;2,"",DAYS360('Features Tracking'!$I15,'Features Tracking'!$J15,FALSE))</f>
         <v>60</v>
       </c>
-      <c r="O15" s="23"/>
-    </row>
-    <row r="16" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O15" s="27">
+        <v>1</v>
+      </c>
+      <c r="P15" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R15" s="21"/>
+      <c r="S15" s="12"/>
+    </row>
+    <row r="16" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" s="13">
         <v>45667</v>
@@ -2050,7 +3010,7 @@
         <v>4</v>
       </c>
       <c r="H16" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E16,'Project Tracking'!$F16)&lt;&gt;2,"",DAYS360('Project Tracking'!$E16,'Project Tracking'!$F16,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E16,'Features Tracking'!$F16)&lt;&gt;2,"",DAYS360('Features Tracking'!$E16,'Features Tracking'!$F16,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I16" s="16">
@@ -2071,20 +3031,30 @@
         <v>0</v>
       </c>
       <c r="N16" s="18">
-        <f>IF(COUNTA('Project Tracking'!$I16,'Project Tracking'!$J16)&lt;&gt;2,"",DAYS360('Project Tracking'!$I16,'Project Tracking'!$J16,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$I16,'Features Tracking'!$J16)&lt;&gt;2,"",DAYS360('Features Tracking'!$I16,'Features Tracking'!$J16,FALSE))</f>
         <v>60</v>
       </c>
-      <c r="O16" s="23"/>
-    </row>
-    <row r="17" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O16" s="27">
+        <v>1</v>
+      </c>
+      <c r="P16" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R16" s="21"/>
+      <c r="S16" s="12"/>
+    </row>
+    <row r="17" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E17" s="13">
         <v>45667</v>
@@ -2096,7 +3066,7 @@
         <v>4</v>
       </c>
       <c r="H17" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E17,'Project Tracking'!$F17)&lt;&gt;2,"",DAYS360('Project Tracking'!$E17,'Project Tracking'!$F17,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E17,'Features Tracking'!$F17)&lt;&gt;2,"",DAYS360('Features Tracking'!$E17,'Features Tracking'!$F17,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I17" s="16">
@@ -2117,20 +3087,30 @@
         <v>0</v>
       </c>
       <c r="N17" s="18">
-        <f>IF(COUNTA('Project Tracking'!$I17,'Project Tracking'!$J17)&lt;&gt;2,"",DAYS360('Project Tracking'!$I17,'Project Tracking'!$J17,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$I17,'Features Tracking'!$J17)&lt;&gt;2,"",DAYS360('Features Tracking'!$I17,'Features Tracking'!$J17,FALSE))</f>
         <v>60</v>
       </c>
-      <c r="O17" s="23"/>
-    </row>
-    <row r="18" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O17" s="27">
+        <v>1</v>
+      </c>
+      <c r="P17" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R17" s="21"/>
+      <c r="S17" s="12"/>
+    </row>
+    <row r="18" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18" s="13">
         <v>45667</v>
@@ -2142,7 +3122,7 @@
         <v>4</v>
       </c>
       <c r="H18" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E18,'Project Tracking'!$F18)&lt;&gt;2,"",DAYS360('Project Tracking'!$E18,'Project Tracking'!$F18,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E18,'Features Tracking'!$F18)&lt;&gt;2,"",DAYS360('Features Tracking'!$E18,'Features Tracking'!$F18,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I18" s="16">
@@ -2163,20 +3143,30 @@
         <v>0</v>
       </c>
       <c r="N18" s="18">
-        <f>IF(COUNTA('Project Tracking'!$I18,'Project Tracking'!$J18)&lt;&gt;2,"",DAYS360('Project Tracking'!$I18,'Project Tracking'!$J18,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$I18,'Features Tracking'!$J18)&lt;&gt;2,"",DAYS360('Features Tracking'!$I18,'Features Tracking'!$J18,FALSE))</f>
         <v>60</v>
       </c>
-      <c r="O18" s="23"/>
-    </row>
-    <row r="19" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O18" s="27">
+        <v>1</v>
+      </c>
+      <c r="P18" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R18" s="21"/>
+      <c r="S18" s="12"/>
+    </row>
+    <row r="19" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E19" s="13">
         <v>45667</v>
@@ -2188,7 +3178,7 @@
         <v>4</v>
       </c>
       <c r="H19" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E19,'Project Tracking'!$F19)&lt;&gt;2,"",DAYS360('Project Tracking'!$E19,'Project Tracking'!$F19,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E19,'Features Tracking'!$F19)&lt;&gt;2,"",DAYS360('Features Tracking'!$E19,'Features Tracking'!$F19,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I19" s="16">
@@ -2209,20 +3199,30 @@
         <v>0</v>
       </c>
       <c r="N19" s="18">
-        <f>IF(COUNTA('Project Tracking'!$I19,'Project Tracking'!$J19)&lt;&gt;2,"",DAYS360('Project Tracking'!$I19,'Project Tracking'!$J19,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$I19,'Features Tracking'!$J19)&lt;&gt;2,"",DAYS360('Features Tracking'!$I19,'Features Tracking'!$J19,FALSE))</f>
         <v>60</v>
       </c>
-      <c r="O19" s="23"/>
-    </row>
-    <row r="20" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O19" s="27">
+        <v>1</v>
+      </c>
+      <c r="P19" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R19" s="21"/>
+      <c r="S19" s="12"/>
+    </row>
+    <row r="20" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E20" s="13">
         <v>45667</v>
@@ -2234,7 +3234,7 @@
         <v>4</v>
       </c>
       <c r="H20" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E20,'Project Tracking'!$F20)&lt;&gt;2,"",DAYS360('Project Tracking'!$E20,'Project Tracking'!$F20,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E20,'Features Tracking'!$F20)&lt;&gt;2,"",DAYS360('Features Tracking'!$E20,'Features Tracking'!$F20,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I20" s="16">
@@ -2255,20 +3255,30 @@
         <v>0</v>
       </c>
       <c r="N20" s="18">
-        <f>IF(COUNTA('Project Tracking'!$I20,'Project Tracking'!$J20)&lt;&gt;2,"",DAYS360('Project Tracking'!$I20,'Project Tracking'!$J20,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$I20,'Features Tracking'!$J20)&lt;&gt;2,"",DAYS360('Features Tracking'!$I20,'Features Tracking'!$J20,FALSE))</f>
         <v>60</v>
       </c>
-      <c r="O20" s="27"/>
-    </row>
-    <row r="21" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O20" s="27">
+        <v>1</v>
+      </c>
+      <c r="P20" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+    </row>
+    <row r="21" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E21" s="13">
         <v>45667</v>
@@ -2280,7 +3290,7 @@
         <v>4</v>
       </c>
       <c r="H21" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E21,'Project Tracking'!$F21)&lt;&gt;2,"",DAYS360('Project Tracking'!$E21,'Project Tracking'!$F21,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E21,'Features Tracking'!$F21)&lt;&gt;2,"",DAYS360('Features Tracking'!$E21,'Features Tracking'!$F21,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I21" s="16">
@@ -2301,20 +3311,30 @@
         <v>0</v>
       </c>
       <c r="N21" s="18">
-        <f>IF(COUNTA('Project Tracking'!$I21,'Project Tracking'!$J21)&lt;&gt;2,"",DAYS360('Project Tracking'!$I21,'Project Tracking'!$J21,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$I21,'Features Tracking'!$J21)&lt;&gt;2,"",DAYS360('Features Tracking'!$I21,'Features Tracking'!$J21,FALSE))</f>
         <v>60</v>
       </c>
-      <c r="O21" s="27"/>
-    </row>
-    <row r="22" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O21" s="27">
+        <v>1</v>
+      </c>
+      <c r="P21" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
+    </row>
+    <row r="22" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E22" s="13">
         <v>45667</v>
@@ -2326,7 +3346,7 @@
         <v>4</v>
       </c>
       <c r="H22" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E22,'Project Tracking'!$F22)&lt;&gt;2,"",DAYS360('Project Tracking'!$E22,'Project Tracking'!$F22,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E22,'Features Tracking'!$F22)&lt;&gt;2,"",DAYS360('Features Tracking'!$E22,'Features Tracking'!$F22,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I22" s="16">
@@ -2347,20 +3367,30 @@
         <v>0</v>
       </c>
       <c r="N22" s="18">
-        <f>IF(COUNTA('Project Tracking'!$I22,'Project Tracking'!$J22)&lt;&gt;2,"",DAYS360('Project Tracking'!$I22,'Project Tracking'!$J22,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$I22,'Features Tracking'!$J22)&lt;&gt;2,"",DAYS360('Features Tracking'!$I22,'Features Tracking'!$J22,FALSE))</f>
         <v>60</v>
       </c>
-      <c r="O22" s="27"/>
-    </row>
-    <row r="23" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O22" s="27">
+        <v>1</v>
+      </c>
+      <c r="P22" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+    </row>
+    <row r="23" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E23" s="13">
         <v>45667</v>
@@ -2372,7 +3402,7 @@
         <v>4</v>
       </c>
       <c r="H23" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E23,'Project Tracking'!$F23)&lt;&gt;2,"",DAYS360('Project Tracking'!$E23,'Project Tracking'!$F23,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E23,'Features Tracking'!$F23)&lt;&gt;2,"",DAYS360('Features Tracking'!$E23,'Features Tracking'!$F23,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I23" s="16">
@@ -2393,20 +3423,30 @@
         <v>0</v>
       </c>
       <c r="N23" s="18">
-        <f>IF(COUNTA('Project Tracking'!$I23,'Project Tracking'!$J23)&lt;&gt;2,"",DAYS360('Project Tracking'!$I23,'Project Tracking'!$J23,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$I23,'Features Tracking'!$J23)&lt;&gt;2,"",DAYS360('Features Tracking'!$I23,'Features Tracking'!$J23,FALSE))</f>
         <v>60</v>
       </c>
-      <c r="O23" s="27"/>
-    </row>
-    <row r="24" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O23" s="27">
+        <v>1</v>
+      </c>
+      <c r="P23" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R23" s="21"/>
+      <c r="S23" s="21"/>
+    </row>
+    <row r="24" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E24" s="13">
         <v>45667</v>
@@ -2418,7 +3458,7 @@
         <v>4</v>
       </c>
       <c r="H24" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E24,'Project Tracking'!$F24)&lt;&gt;2,"",DAYS360('Project Tracking'!$E24,'Project Tracking'!$F24,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E24,'Features Tracking'!$F24)&lt;&gt;2,"",DAYS360('Features Tracking'!$E24,'Features Tracking'!$F24,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I24" s="16">
@@ -2439,20 +3479,30 @@
         <v>0</v>
       </c>
       <c r="N24" s="18">
-        <f>IF(COUNTA('Project Tracking'!$I24,'Project Tracking'!$J24)&lt;&gt;2,"",DAYS360('Project Tracking'!$I24,'Project Tracking'!$J24,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$I24,'Features Tracking'!$J24)&lt;&gt;2,"",DAYS360('Features Tracking'!$I24,'Features Tracking'!$J24,FALSE))</f>
         <v>60</v>
       </c>
-      <c r="O24" s="27"/>
-    </row>
-    <row r="25" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O24" s="27">
+        <v>1</v>
+      </c>
+      <c r="P24" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R24" s="21"/>
+      <c r="S24" s="21"/>
+    </row>
+    <row r="25" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E25" s="13">
         <v>45667</v>
@@ -2464,7 +3514,7 @@
         <v>4</v>
       </c>
       <c r="H25" s="15">
-        <f>IF(COUNTA('Project Tracking'!$E25,'Project Tracking'!$F25)&lt;&gt;2,"",DAYS360('Project Tracking'!$E25,'Project Tracking'!$F25,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$E25,'Features Tracking'!$F25)&lt;&gt;2,"",DAYS360('Features Tracking'!$E25,'Features Tracking'!$F25,FALSE))</f>
         <v>30</v>
       </c>
       <c r="I25" s="16">
@@ -2485,20 +3535,30 @@
         <v>0</v>
       </c>
       <c r="N25" s="18">
-        <f>IF(COUNTA('Project Tracking'!$I25,'Project Tracking'!$J25)&lt;&gt;2,"",DAYS360('Project Tracking'!$I25,'Project Tracking'!$J25,FALSE))</f>
+        <f>IF(COUNTA('Features Tracking'!$I25,'Features Tracking'!$J25)&lt;&gt;2,"",DAYS360('Features Tracking'!$I25,'Features Tracking'!$J25,FALSE))</f>
         <v>60</v>
       </c>
-      <c r="O25" s="27"/>
+      <c r="O25" s="27">
+        <v>1</v>
+      </c>
+      <c r="P25" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="L5:L25">
-    <cfRule type="expression" dxfId="1" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>(ABS((L5-G5))/G5)&gt;FlagPercent</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5:N25">
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>(ABS((N5-H5))/H5)&gt;FlagPercent</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2520,7 +3580,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Biểu tượng Cờ ở đầu đề bảng Bộ theo dõi Dự án cho Thời gian Thực Trên/Dưới (Giá trị theo ngày trong cột N đáp ứng tiêu chí Trên/Dưới sẽ tạo một biểu tượng cờ trong mỗi ô ở cột này. Các ô trống cho biết giá trị không đáp ứng tiêu chí Trên/Dưới" sqref="M4" xr:uid="{00000000-0002-0000-0000-000010000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Hãy nhập lượng công việc thực tế của dự án tính theo giờ. Các giá trị đáp ứng tiêu chí Trên/Dưới sẽ được tô đậm bằng màu đỏ và tạo ra một biểu tượng gắn cờ trong cột K ở bên trái" sqref="L4" xr:uid="{00000000-0002-0000-0000-000011000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Hãy nhập khoảng thời gian thực tế của dự án tính theo ngày. Các giá trị đáp ứng tiêu chí Trên/Dưới sẽ được tô đậm bằng màu đỏ và tạo biểu tượng gắn cờ trong cột M ở bên trái" sqref="N4" xr:uid="{00000000-0002-0000-0000-000012000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ghi chú cho dự án ở cột này" sqref="O4" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ghi chú cho dự án ở cột này" sqref="O4:R4" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -2574,21 +3634,538 @@
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="50" yWindow="402" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{68EBA7E1-E12E-42E6-8B40-BF7D31B68A37}">
+          <x14:formula1>
+            <xm:f>Setting!$F$5:$F$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>O5:O25</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6AAF1592-527B-4237-81B4-E288732AEB87}">
+          <x14:formula1>
+            <xm:f>Setting!$I$5:$I$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>P5:P25</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EEBF197F-BBCD-43A2-BC23-F330D35146E7}">
+          <x14:formula1>
+            <xm:f>Setting!$L$5:$L$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q5:Q25</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB65F83-37E0-4DB5-93DD-F7DA85C794B8}">
+  <sheetPr>
+    <tabColor theme="9"/>
+    <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:S25"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.69921875" style="1" customWidth="1"/>
+    <col min="2" max="4" width="22.59765625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="15.59765625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.59765625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.796875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="15.59765625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="2.796875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="14.09765625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="2.796875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.3984375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.796875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.09765625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15.296875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21.3984375" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="5">
+        <f>COUNTIF(Q5:Q8,"Yes")/COUNTA(Q5:Q8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:19" ht="54.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="13">
+        <v>45667</v>
+      </c>
+      <c r="F5" s="13">
+        <v>45698</v>
+      </c>
+      <c r="G5" s="14">
+        <v>4</v>
+      </c>
+      <c r="H5" s="15">
+        <f>IF(COUNTA('External Module Tracking'!$E5,'External Module Tracking'!$F5)&lt;&gt;2,"",DAYS360('External Module Tracking'!$E5,'External Module Tracking'!$F5,FALSE))</f>
+        <v>30</v>
+      </c>
+      <c r="I5" s="16">
+        <f ca="1">TODAY()-65</f>
+        <v>45631</v>
+      </c>
+      <c r="J5" s="13">
+        <f ca="1">TODAY()</f>
+        <v>45696</v>
+      </c>
+      <c r="K5" s="17">
+        <f>IFERROR(IF(Bộ_theo_dõi_Dự_án7[[#This Row],[Actual amount of time]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án7[[#This Row],[Actual amount of time]]-Bộ_theo_dõi_Dự_án7[[#This Row],[Planned amount of time]])/Bộ_theo_dõi_Dự_án7[[#This Row],[Planned amount of time]])&gt;FlagPercent,1,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="L5" s="14">
+        <v>300</v>
+      </c>
+      <c r="M5" s="17">
+        <f ca="1">IFERROR(IF(Bộ_theo_dõi_Dự_án7[[#This Row],[Actual number of days]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án7[[#This Row],[Actual number of days]]-Bộ_theo_dõi_Dự_án7[[#This Row],[Planned number of days]])/Bộ_theo_dõi_Dự_án7[[#This Row],[Planned number of days]])&gt;FlagPercent,1,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="N5" s="18">
+        <f ca="1">IF(COUNTA('External Module Tracking'!$I5,'External Module Tracking'!$J5)&lt;&gt;2,"",DAYS360('External Module Tracking'!$I5,'External Module Tracking'!$J5,FALSE))</f>
+        <v>63</v>
+      </c>
+      <c r="O5" s="27">
+        <v>1</v>
+      </c>
+      <c r="P5" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R5" s="21"/>
+      <c r="S5" s="12"/>
+    </row>
+    <row r="6" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="13">
+        <v>45667</v>
+      </c>
+      <c r="F6" s="13">
+        <v>45698</v>
+      </c>
+      <c r="G6" s="14">
+        <v>4</v>
+      </c>
+      <c r="H6" s="15">
+        <f>IF(COUNTA('External Module Tracking'!$E6,'External Module Tracking'!$F6)&lt;&gt;2,"",DAYS360('External Module Tracking'!$E6,'External Module Tracking'!$F6,FALSE))</f>
+        <v>30</v>
+      </c>
+      <c r="I6" s="16">
+        <f ca="1">TODAY()-41</f>
+        <v>45655</v>
+      </c>
+      <c r="J6" s="13">
+        <f ca="1">TODAY()-7</f>
+        <v>45689</v>
+      </c>
+      <c r="K6" s="17">
+        <f>IFERROR(IF(Bộ_theo_dõi_Dự_án7[[#This Row],[Actual amount of time]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án7[[#This Row],[Actual amount of time]]-Bộ_theo_dõi_Dự_án7[[#This Row],[Planned amount of time]])/Bộ_theo_dõi_Dự_án7[[#This Row],[Planned amount of time]])&gt;FlagPercent,1,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="L6" s="14">
+        <v>390</v>
+      </c>
+      <c r="M6" s="17">
+        <f ca="1">IFERROR(IF(Bộ_theo_dõi_Dự_án7[[#This Row],[Actual number of days]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án7[[#This Row],[Actual number of days]]-Bộ_theo_dõi_Dự_án7[[#This Row],[Planned number of days]])/Bộ_theo_dõi_Dự_án7[[#This Row],[Planned number of days]])&gt;FlagPercent,1,0)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="18">
+        <f ca="1">IF(COUNTA('External Module Tracking'!$I6,'External Module Tracking'!$J6)&lt;&gt;2,"",DAYS360('External Module Tracking'!$I6,'External Module Tracking'!$J6,FALSE))</f>
+        <v>32</v>
+      </c>
+      <c r="O6" s="27">
+        <v>1</v>
+      </c>
+      <c r="P6" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R6" s="21"/>
+      <c r="S6" s="12"/>
+    </row>
+    <row r="7" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="13">
+        <v>45667</v>
+      </c>
+      <c r="F7" s="13">
+        <v>45698</v>
+      </c>
+      <c r="G7" s="14">
+        <v>4</v>
+      </c>
+      <c r="H7" s="15">
+        <f>IF(COUNTA('External Module Tracking'!$E7,'External Module Tracking'!$F7)&lt;&gt;2,"",DAYS360('External Module Tracking'!$E7,'External Module Tracking'!$F7,FALSE))</f>
+        <v>30</v>
+      </c>
+      <c r="I7" s="16">
+        <f ca="1">TODAY()-100</f>
+        <v>45596</v>
+      </c>
+      <c r="J7" s="13">
+        <f ca="1">TODAY()-27</f>
+        <v>45669</v>
+      </c>
+      <c r="K7" s="17">
+        <f>IFERROR(IF(Bộ_theo_dõi_Dự_án7[[#This Row],[Actual amount of time]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án7[[#This Row],[Actual amount of time]]-Bộ_theo_dõi_Dự_án7[[#This Row],[Planned amount of time]])/Bộ_theo_dõi_Dự_án7[[#This Row],[Planned amount of time]])&gt;FlagPercent,1,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="L7" s="14">
+        <v>500</v>
+      </c>
+      <c r="M7" s="17">
+        <f ca="1">IFERROR(IF(Bộ_theo_dõi_Dự_án7[[#This Row],[Actual number of days]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án7[[#This Row],[Actual number of days]]-Bộ_theo_dõi_Dự_án7[[#This Row],[Planned number of days]])/Bộ_theo_dõi_Dự_án7[[#This Row],[Planned number of days]])&gt;FlagPercent,1,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="N7" s="18">
+        <f ca="1">IF(COUNTA('External Module Tracking'!$I7,'External Module Tracking'!$J7)&lt;&gt;2,"",DAYS360('External Module Tracking'!$I7,'External Module Tracking'!$J7,FALSE))</f>
+        <v>72</v>
+      </c>
+      <c r="O7" s="27">
+        <v>1</v>
+      </c>
+      <c r="P7" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R7" s="21"/>
+      <c r="S7" s="12"/>
+    </row>
+    <row r="8" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="13">
+        <v>45667</v>
+      </c>
+      <c r="F8" s="13">
+        <v>45698</v>
+      </c>
+      <c r="G8" s="14">
+        <v>4</v>
+      </c>
+      <c r="H8" s="15">
+        <f>IF(COUNTA('External Module Tracking'!$E8,'External Module Tracking'!$F8)&lt;&gt;2,"",DAYS360('External Module Tracking'!$E8,'External Module Tracking'!$F8,FALSE))</f>
+        <v>30</v>
+      </c>
+      <c r="I8" s="16">
+        <f ca="1">TODAY()-90</f>
+        <v>45606</v>
+      </c>
+      <c r="J8" s="13">
+        <f ca="1">TODAY()-71</f>
+        <v>45625</v>
+      </c>
+      <c r="K8" s="17">
+        <f>IFERROR(IF(Bộ_theo_dõi_Dự_án7[[#This Row],[Actual amount of time]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án7[[#This Row],[Actual amount of time]]-Bộ_theo_dõi_Dự_án7[[#This Row],[Planned amount of time]])/Bộ_theo_dõi_Dự_án7[[#This Row],[Planned amount of time]])&gt;FlagPercent,1,0)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="L8" s="14">
+        <v>276</v>
+      </c>
+      <c r="M8" s="17">
+        <f ca="1">IFERROR(IF(Bộ_theo_dõi_Dự_án7[[#This Row],[Actual number of days]]=0,"",IF(ABS((Bộ_theo_dõi_Dự_án7[[#This Row],[Actual number of days]]-Bộ_theo_dõi_Dự_án7[[#This Row],[Planned number of days]])/Bộ_theo_dõi_Dự_án7[[#This Row],[Planned number of days]])&gt;FlagPercent,1,0)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="18">
+        <f ca="1">IF(COUNTA('External Module Tracking'!$I8,'External Module Tracking'!$J8)&lt;&gt;2,"",DAYS360('External Module Tracking'!$I8,'External Module Tracking'!$J8,FALSE))</f>
+        <v>19</v>
+      </c>
+      <c r="O8" s="27">
+        <v>1</v>
+      </c>
+      <c r="P8" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R8" s="21"/>
+      <c r="S8" s="12"/>
+    </row>
+    <row r="9" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S9" s="12"/>
+    </row>
+    <row r="10" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S10" s="12"/>
+    </row>
+    <row r="11" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S11" s="12"/>
+    </row>
+    <row r="12" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S12" s="12"/>
+    </row>
+    <row r="13" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S13" s="12"/>
+    </row>
+    <row r="14" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S14" s="12"/>
+    </row>
+    <row r="15" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S15" s="12"/>
+    </row>
+    <row r="16" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S16" s="12"/>
+    </row>
+    <row r="17" spans="19:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S17" s="12"/>
+    </row>
+    <row r="18" spans="19:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S18" s="12"/>
+    </row>
+    <row r="19" spans="19:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S19" s="12"/>
+    </row>
+    <row r="20" spans="19:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S20" s="21"/>
+    </row>
+    <row r="21" spans="19:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S21" s="21"/>
+    </row>
+    <row r="22" spans="19:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S22" s="21"/>
+    </row>
+    <row r="23" spans="19:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S23" s="21"/>
+    </row>
+    <row r="24" spans="19:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S24" s="21"/>
+    </row>
+    <row r="25" spans="19:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S25" s="21"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="L5:L8">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>(ABS((L5-G5))/G5)&gt;FlagPercent</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5:N8">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>(ABS((N5-H5))/H5)&gt;FlagPercent</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="16">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ghi chú cho dự án ở cột này" sqref="O4:R4" xr:uid="{794E30B9-9FE1-45A8-8A62-388DD459718A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Hãy nhập khoảng thời gian thực tế của dự án tính theo ngày. Các giá trị đáp ứng tiêu chí Trên/Dưới sẽ được tô đậm bằng màu đỏ và tạo biểu tượng gắn cờ trong cột M ở bên trái" sqref="N4" xr:uid="{89D76462-25EB-40DE-B0EA-DD3BCA51496B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Hãy nhập lượng công việc thực tế của dự án tính theo giờ. Các giá trị đáp ứng tiêu chí Trên/Dưới sẽ được tô đậm bằng màu đỏ và tạo ra một biểu tượng gắn cờ trong cột K ở bên trái" sqref="L4" xr:uid="{E3351820-B12C-463B-979C-451103E6E7F4}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Biểu tượng Cờ ở đầu đề bảng Bộ theo dõi Dự án cho Thời gian Thực Trên/Dưới (Giá trị theo ngày trong cột N đáp ứng tiêu chí Trên/Dưới sẽ tạo một biểu tượng cờ trong mỗi ô ở cột này. Các ô trống cho biết giá trị không đáp ứng tiêu chí Trên/Dưới" sqref="M4" xr:uid="{299BB405-C653-495B-BC19-68937A177F10}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Biểu tượng Cờ ở đầu đề bảng Bộ theo dõi Dự án cho Công việc Thực Trên/Dưới (theo giờ). Các giá trị trong cột L đáp ứng tiêu chí Trên/Dưới sẽ tạo một biểu tượng cờ trong mỗi ô ở cột này. Các ô trống cho biết giá trị không đáp ứng tiêu chí Trên/Dưới" sqref="K4" xr:uid="{9D486CEC-1CEB-4D27-A54A-28F488D8DB00}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày hoàn thành dự án thực tế vào cột này" sqref="J4" xr:uid="{05C5E274-4CF2-4A45-BE66-87B7D42DD8F5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày bắt đầu dự án thực tế vào cột này" sqref="I4" xr:uid="{AA8160F9-90C5-487C-80D5-03A3514D7311}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập khoảng thời gian dự kiến cho dự án tính theo ngày vào cột này" sqref="H4" xr:uid="{F015BBF8-4081-4613-B899-62E7764F83E7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập lượng công việc dự kiến cho dự án tính theo giờ" sqref="G4" xr:uid="{9D7103BF-1BE2-44C3-82A4-4D8744B519B2}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày hoàn thành dự án dự kiến vào cột này" sqref="F4" xr:uid="{3650F7E1-6E46-4090-9A99-92493191C50C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày bắt đầu dự án dự kiến vào cột này" sqref="E4" xr:uid="{95FCF388-4641-4F3C-8340-C3303B2BFA82}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Chọn tên Nhân viên từ danh sách thả xuống trong từng ô ở cột này. Các tùy chọn sẽ được xác định trong trang tính Thiết lập. Nhấn ALT + MŨI TÊN XUỐNG để dẫn hướng trong danh sách, rồi nhấn ENTER để lựa chọn" sqref="D4" xr:uid="{1A4BC614-7FD0-46FC-AE02-C129EF4DCAC1}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập tên dự án vào cột này" sqref="B4:C4" xr:uid="{85769808-F7F8-4EDE-AD81-5245B2B54693}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Chọn một nhân viên từ danh sách hoặc tạo một nhân viên mới để hiển thị trong danh sách này từ trang tính Thiết lập." sqref="D5:D8" xr:uid="{EB5DE53F-A25A-4A5F-BFDE-BAD19845D845}">
+      <formula1>EmployeeList</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phần trăm trên/dưới có thể tùy chỉnh được dùng để tô sáng công việc thực tế tính theo giờ và ngày trong bảng dự án vượt quá hạn hoặc ở dưới con số này" sqref="D2" xr:uid="{08DAE562-20D5-489E-9423-531DC6519D2C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" prompt="Nhập dự án vào trang tính bộ theo dõi dự án này. Đặt phần trăm trên/dưới để gắn cờ trong D2. Công việc thực tính theo giờ và thời gian thực tính theo ngày sẽ tô sáng giá trị trên/dưới với kiểu phông chữ đậm, đỏ và biểu tượng cờ trong các cột K và M" sqref="A1" xr:uid="{7EFA52FA-F11B-4086-B45E-9ECDCEDA3328}"/>
+  </dataValidations>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <headerFooter differentFirst="1">
+    <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="25" id="{1B5D935C-19AF-4728-A8C4-150009315B11}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K5:K8</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="27" id="{8E53D9FF-8ADF-469E-B0FC-AAB31013A499}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>M5:M8</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4B26A858-72A4-46D2-8E77-335C709A4CFF}">
+          <x14:formula1>
+            <xm:f>Setting!$L$5:$L$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q5:Q8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DE6ED132-2B49-478B-850E-437BD75EB9E5}">
+          <x14:formula1>
+            <xm:f>Setting!$I$5:$I$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>P5:P8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F0332E62-255B-438A-AAA2-1847876C153A}">
+          <x14:formula1>
+            <xm:f>Setting!$F$5:$F$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>O5:O8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2">
     <tabColor theme="3"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:C11"/>
+  <dimension ref="B1:M11"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2596,53 +4173,169 @@
     <col min="1" max="1" width="2.69921875" style="1" customWidth="1"/>
     <col min="2" max="3" width="25.59765625" style="1" customWidth="1"/>
     <col min="4" max="4" width="2.69921875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="1"/>
+    <col min="5" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="24.69921875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.3984375" style="1" customWidth="1"/>
+    <col min="8" max="9" width="9" style="1"/>
+    <col min="10" max="10" width="27.296875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.3984375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.09765625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="25"/>
-    </row>
-    <row r="3" spans="2:3" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="24"/>
+    </row>
+    <row r="3" spans="2:13" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="L3" s="26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="21">
+        <v>0</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="21">
+        <v>0</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="L5" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="22"/>
-    </row>
-    <row r="11" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="27">
+        <v>0.25</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="27">
+        <v>0.25</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="M6" s="21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="27">
+        <v>0.75</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="27">
+        <v>0.75</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="27">
+        <v>1</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="27">
+        <v>1</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="22"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" prompt="Trang tính thiết lập có chứa danh sách các danh mục dự án và tên nhân viên có thể tùy chỉnh. Những danh sách này được sử dụng dưới dạng danh sách thả xuống trong trang tính của bộ theo dõi dự án. Các danh sách không cần phải có cùng số mục " sqref="A1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập tên nhân viên vào cột này, cột được dùng làm tùy chọn trong danh sách thả xuống Đã gán Cho ở trang tính Bộ theo dõi Dự án" sqref="B4" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập tên nhân viên vào cột này, cột được dùng làm tùy chọn trong danh sách thả xuống Đã gán Cho ở trang tính Bộ theo dõi Dự án" sqref="B4 F4:F5 I4:I5 L4" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>